<commit_message>
Actualización datos por regiones
Actualización de datos.
</commit_message>
<xml_diff>
--- a/Proyectos/G5_Bian_Ortiz_Monzon/inflacion_regiones.xlsx
+++ b/Proyectos/G5_Bian_Ortiz_Monzon/inflacion_regiones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN_CAP02\Documents\Curso R - BABS -\Proyecto grupal\Reporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A025EF8-4D29-47AE-B687-4E54D35FDA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7098752E-762E-435F-BF60-423B3EB9A111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6ABC1709-5FBF-4255-A2DE-B03C80689CF6}"/>
   </bookViews>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA57BEAD-7330-4CD4-BE7A-374DC11A4F9F}">
   <dimension ref="A1:K298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
-      <selection activeCell="A303" sqref="A303"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="I295" sqref="I295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10672,31 +10672,31 @@
         <v>2</v>
       </c>
       <c r="C290" s="10">
-        <v>101.017579223309</v>
+        <v>100.80654436022658</v>
       </c>
       <c r="D290" s="9">
-        <v>100.440988114646</v>
+        <v>100.41388529125275</v>
       </c>
       <c r="E290" s="9">
-        <v>101.573799813579</v>
+        <v>100.88036396691089</v>
       </c>
       <c r="F290" s="9">
-        <v>100.747482136363</v>
+        <v>100.97719362004808</v>
       </c>
       <c r="G290" s="9">
-        <v>100.730879048418</v>
+        <v>100.63915448922428</v>
       </c>
       <c r="H290" s="9">
-        <v>101.289745367872</v>
+        <v>101.19325791651227</v>
       </c>
       <c r="I290" s="9">
-        <v>100.814906669115</v>
+        <v>100.74607051077707</v>
       </c>
       <c r="J290" s="9">
-        <v>101.67884942791299</v>
+        <v>101.12377052788172</v>
       </c>
       <c r="K290" s="9">
-        <v>101.131068948007</v>
+        <v>100.87921461774297</v>
       </c>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.25">
@@ -10707,31 +10707,31 @@
         <v>3</v>
       </c>
       <c r="C291" s="10">
-        <v>100.76650710231</v>
+        <v>100.56907758478992</v>
       </c>
       <c r="D291" s="9">
-        <v>100.54764119971701</v>
+        <v>100.53358581407466</v>
       </c>
       <c r="E291" s="9">
-        <v>101.148438516494</v>
+        <v>100.47097464898768</v>
       </c>
       <c r="F291" s="9">
-        <v>100.407447333916</v>
+        <v>100.64947480416981</v>
       </c>
       <c r="G291" s="9">
-        <v>100.28808185486599</v>
+        <v>100.2097946044064</v>
       </c>
       <c r="H291" s="9">
-        <v>101.112678600897</v>
+        <v>101.02950054085503</v>
       </c>
       <c r="I291" s="9">
-        <v>100.424091577719</v>
+        <v>100.36857702136638</v>
       </c>
       <c r="J291" s="9">
-        <v>101.41977278521</v>
+        <v>100.87922939445306</v>
       </c>
       <c r="K291" s="9">
-        <v>100.714695725087</v>
+        <v>100.47694717042354</v>
       </c>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.25">
@@ -10742,31 +10742,31 @@
         <v>4</v>
       </c>
       <c r="C292" s="10">
-        <v>100.862479384954</v>
+        <v>100.69255321166003</v>
       </c>
       <c r="D292" s="10">
-        <v>100.729180919325</v>
+        <v>100.74280535688288</v>
       </c>
       <c r="E292" s="9">
-        <v>101.245716140398</v>
+        <v>100.59526536012748</v>
       </c>
       <c r="F292" s="9">
-        <v>100.55430770853199</v>
+        <v>100.8244168231094</v>
       </c>
       <c r="G292" s="10">
-        <v>100.40622001960701</v>
+        <v>100.35543921877249</v>
       </c>
       <c r="H292" s="10">
-        <v>100.98391906176001</v>
+        <v>100.92860321930067</v>
       </c>
       <c r="I292" s="10">
-        <v>100.453264335642</v>
+        <v>100.42535155016287</v>
       </c>
       <c r="J292" s="10">
-        <v>101.565417294271</v>
+        <v>101.0518878536122</v>
       </c>
       <c r="K292" s="10">
-        <v>100.852854532039</v>
+        <v>100.64245744144543</v>
       </c>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.25">
@@ -10777,31 +10777,31 @@
         <v>5</v>
       </c>
       <c r="C293" s="10">
-        <v>101.058686802872</v>
+        <v>100.93199241206872</v>
       </c>
       <c r="D293" s="10">
-        <v>100.896600823966</v>
+        <v>100.9538194500626</v>
       </c>
       <c r="E293" s="9">
-        <v>101.556322224018</v>
+        <v>100.94744478343137</v>
       </c>
       <c r="F293" s="9">
-        <v>100.68000409132701</v>
+        <v>100.9940404647308</v>
       </c>
       <c r="G293" s="10">
-        <v>100.643631942879</v>
+        <v>100.63616576973648</v>
       </c>
       <c r="H293" s="10">
-        <v>101.25999832321099</v>
+        <v>101.24822963417799</v>
       </c>
       <c r="I293" s="10">
-        <v>100.555971489744</v>
+        <v>100.57143728960307</v>
       </c>
       <c r="J293" s="10">
-        <v>101.730562459361</v>
+        <v>101.25990199261206</v>
       </c>
       <c r="K293" s="10">
-        <v>101.06344428053301</v>
+        <v>100.89615451240682</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.25">
@@ -10812,31 +10812,31 @@
         <v>6</v>
       </c>
       <c r="C294" s="10">
-        <v>101.306106231022</v>
+        <v>101.22205562988458</v>
       </c>
       <c r="D294" s="10">
-        <v>101.05225620583801</v>
+        <v>101.15248777192294</v>
       </c>
       <c r="E294" s="10">
-        <v>101.891652100776</v>
+        <v>101.32376152094358</v>
       </c>
       <c r="F294" s="10">
-        <v>100.919528568286</v>
+        <v>101.27728897092486</v>
       </c>
       <c r="G294" s="10">
-        <v>100.739946316317</v>
+        <v>100.77523732197081</v>
       </c>
       <c r="H294" s="10">
-        <v>101.580815361313</v>
+        <v>101.61212933586118</v>
       </c>
       <c r="I294" s="10">
-        <v>100.72914000103999</v>
+        <v>100.78740155798899</v>
       </c>
       <c r="J294" s="10">
-        <v>102.198494687805</v>
+        <v>101.76885521602804</v>
       </c>
       <c r="K294" s="10">
-        <v>101.33541705398299</v>
+        <v>101.21062643506568</v>
       </c>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.25">
@@ -10847,31 +10847,31 @@
         <v>7</v>
       </c>
       <c r="C295" s="10">
-        <v>101.56274012722299</v>
+        <v>101.50946460471643</v>
       </c>
       <c r="D295" s="10">
-        <v>101.36169601274899</v>
+        <v>101.49321771956062</v>
       </c>
       <c r="E295" s="10">
-        <v>102.245543025663</v>
+        <v>101.70672819482401</v>
       </c>
       <c r="F295" s="10">
-        <v>101.13852903760601</v>
+        <v>101.52805955517674</v>
       </c>
       <c r="G295" s="10">
-        <v>100.992690081411</v>
+        <v>101.05892013966746</v>
       </c>
       <c r="H295" s="10">
-        <v>101.714379626118</v>
+        <v>101.77680502295046</v>
       </c>
       <c r="I295" s="10">
-        <v>101.043994203404</v>
+        <v>101.13331075941143</v>
       </c>
       <c r="J295" s="10">
-        <v>102.39833001485</v>
+        <v>101.9989883102853</v>
       </c>
       <c r="K295" s="10">
-        <v>101.599471068376</v>
+        <v>101.50534173043036</v>
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.25">
@@ -10882,31 +10882,31 @@
         <v>8</v>
       </c>
       <c r="C296" s="10">
-        <v>101.81200043071399</v>
+        <v>101.90563096792266</v>
       </c>
       <c r="D296" s="10">
-        <v>101.578475123478</v>
+        <v>101.85724495061937</v>
       </c>
       <c r="E296" s="10">
-        <v>102.742520595644</v>
+        <v>102.34876321885635</v>
       </c>
       <c r="F296" s="10">
-        <v>101.445609040848</v>
+        <v>101.98347220239677</v>
       </c>
       <c r="G296" s="10">
-        <v>101.309940312587</v>
+        <v>101.52286339052453</v>
       </c>
       <c r="H296" s="10">
-        <v>101.840940201265</v>
+        <v>102.05068949102518</v>
       </c>
       <c r="I296" s="10">
-        <v>101.224680359088</v>
+        <v>101.46055220176935</v>
       </c>
       <c r="J296" s="10">
-        <v>102.575002850799</v>
+        <v>102.32261022972659</v>
       </c>
       <c r="K296" s="10">
-        <v>101.90663606807099</v>
+        <v>101.95933671288608</v>
       </c>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.25">
@@ -10917,31 +10917,31 @@
         <v>9</v>
       </c>
       <c r="C297" s="10">
-        <v>101.752936088523</v>
+        <v>101.81547901296761</v>
       </c>
       <c r="D297" s="10">
-        <v>101.417823487729</v>
+        <v>101.6651649299793</v>
       </c>
       <c r="E297" s="10">
-        <v>102.963274515633</v>
+        <v>102.53741759475174</v>
       </c>
       <c r="F297" s="10">
-        <v>101.356388074237</v>
+        <v>101.86272959674228</v>
       </c>
       <c r="G297" s="10">
-        <v>101.24168885250199</v>
+        <v>101.42355415538803</v>
       </c>
       <c r="H297" s="10">
-        <v>101.78370927408299</v>
+        <v>101.96226191269749</v>
       </c>
       <c r="I297" s="10">
-        <v>101.071720028914</v>
+        <v>101.27636580425535</v>
       </c>
       <c r="J297" s="10">
-        <v>102.55202581314001</v>
+        <v>102.26851828736902</v>
       </c>
       <c r="K297" s="10">
-        <v>101.848010915171</v>
+        <v>101.86963146930056</v>
       </c>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>